<commit_message>
Creates tables for CNES and Municipio frequencies. Groups the network in General network and Surgery network
</commit_message>
<xml_diff>
--- a/output/freq_idades.xlsx
+++ b/output/freq_idades.xlsx
@@ -496,7 +496,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="n">
         <v>513</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B8" t="n">
         <v>513</v>

</xml_diff>